<commit_message>
fixed typos in templates
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_сводная.xlsx
+++ b/templates/ведомость_курсанты_сводная.xlsx
@@ -48,9 +48,6 @@
     <t>Фамилия Имя Отчество</t>
   </si>
   <si>
-    <t>Оценка на котрольных занятиях</t>
-  </si>
-  <si>
     <t>СП</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>Дата сдачи: «___» $month$ $year$ года</t>
+  </si>
+  <si>
+    <t>Оценка на контрольных занятиях</t>
   </si>
 </sst>
 </file>
@@ -665,8 +665,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:L959"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
     </row>
     <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -726,7 +726,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -742,7 +742,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
@@ -781,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -789,13 +789,13 @@
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="L7" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -803,22 +803,22 @@
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
@@ -829,10 +829,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -930,7 +930,7 @@
     </row>
     <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>

</xml_diff>